<commit_message>
Model updated : adding loss plot and retrained
</commit_message>
<xml_diff>
--- a/src/results.xlsx
+++ b/src/results.xlsx
@@ -377,7 +377,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C352"/>
+  <dimension ref="A1:C365"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -396,10 +396,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>291.70849609375</v>
+        <v>500.1842956542969</v>
       </c>
       <c r="C2">
-        <v>294.1023864746094</v>
+        <v>503.2980041503906</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -407,10 +407,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>332.1370849609375</v>
+        <v>383.9866027832032</v>
       </c>
       <c r="C3">
-        <v>311.3477783203125</v>
+        <v>396.2442932128906</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -418,10 +418,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>326.7294921875</v>
+        <v>255.3294982910156</v>
       </c>
       <c r="C4">
-        <v>316.7756042480469</v>
+        <v>247.2734985351562</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -429,10 +429,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>270.598388671875</v>
+        <v>332.1370849609375</v>
       </c>
       <c r="C5">
-        <v>275.6035461425781</v>
+        <v>299.3583068847656</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -440,10 +440,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>497.0021057128906</v>
+        <v>295.3533935546875</v>
       </c>
       <c r="C6">
-        <v>505.6777648925781</v>
+        <v>296.5397644042969</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -451,10 +451,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>403.2861022949219</v>
+        <v>498.7203063964844</v>
       </c>
       <c r="C7">
-        <v>400.4152526855469</v>
+        <v>510.0304870605469</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -462,10 +462,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>522.5180053710938</v>
+        <v>280.3630065917969</v>
       </c>
       <c r="C8">
-        <v>519.38623046875</v>
+        <v>263.2757568359375</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -473,10 +473,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>402.9413146972656</v>
+        <v>403.1365051269531</v>
       </c>
       <c r="C9">
-        <v>410.6878356933594</v>
+        <v>399.2208251953125</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -484,10 +484,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>430.14111328125</v>
+        <v>514.4263916015625</v>
       </c>
       <c r="C10">
-        <v>424.1364440917969</v>
+        <v>516.8399658203125</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -495,10 +495,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>518.2965698242188</v>
+        <v>404.5138854980468</v>
       </c>
       <c r="C11">
-        <v>513.6127319335938</v>
+        <v>392.0443420410156</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -506,10 +506,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>261.2950134277344</v>
+        <v>301.095703125</v>
       </c>
       <c r="C12">
-        <v>276.1006774902344</v>
+        <v>290.5632934570312</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -517,10 +517,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>278.8116149902344</v>
+        <v>301.6788940429688</v>
       </c>
       <c r="C13">
-        <v>271.0606079101562</v>
+        <v>281.3732299804688</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -528,10 +528,10 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>314.0155029296875</v>
+        <v>275</v>
       </c>
       <c r="C14">
-        <v>328.0509948730469</v>
+        <v>255.1671447753906</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -539,10 +539,10 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>255.3294982910156</v>
+        <v>402.2528076171876</v>
       </c>
       <c r="C15">
-        <v>261.6921997070312</v>
+        <v>393.8383178710938</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -550,10 +550,10 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>419.1980895996094</v>
+        <v>367.9718933105469</v>
       </c>
       <c r="C16">
-        <v>428.9523620605469</v>
+        <v>362.6744079589844</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -561,10 +561,10 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>492.1051025390625</v>
+        <v>438.0693969726562</v>
       </c>
       <c r="C17">
-        <v>481.1339721679688</v>
+        <v>426.41552734375</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -572,10 +572,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>304.0939025878906</v>
+        <v>293.1224975585938</v>
       </c>
       <c r="C18">
-        <v>304.1192321777344</v>
+        <v>273.2843627929688</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -583,10 +583,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>277.6722106933594</v>
+        <v>445.1534118652344</v>
       </c>
       <c r="C19">
-        <v>271.7694396972656</v>
+        <v>429.0836486816406</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -594,10 +594,10 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>408.119384765625</v>
+        <v>299.3187866210938</v>
       </c>
       <c r="C20">
-        <v>416.4229125976562</v>
+        <v>286.8689575195312</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -605,10 +605,10 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>420.7026062011719</v>
+        <v>392.2799987792969</v>
       </c>
       <c r="C21">
-        <v>419.699951171875</v>
+        <v>394.5169372558594</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -616,10 +616,10 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>252.6526031494141</v>
+        <v>358.076904296875</v>
       </c>
       <c r="C22">
-        <v>268.0166931152344</v>
+        <v>363.6390075683594</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -627,10 +627,10 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>292.2999877929688</v>
+        <v>292.4132995605469</v>
       </c>
       <c r="C23">
-        <v>278.0745849609375</v>
+        <v>270.3749084472656</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -638,10 +638,10 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>389.7925109863281</v>
+        <v>572.4967041015625</v>
       </c>
       <c r="C24">
-        <v>405.1939697265625</v>
+        <v>574.6187133789062</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -649,10 +649,10 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>344.9400024414062</v>
+        <v>273.8634033203125</v>
       </c>
       <c r="C25">
-        <v>350.3557434082031</v>
+        <v>249.0012664794922</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -660,10 +660,10 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>401.9627075195313</v>
+        <v>544.2470092773438</v>
       </c>
       <c r="C26">
-        <v>415.4222106933594</v>
+        <v>530.888916015625</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -671,10 +671,10 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>417.4896850585938</v>
+        <v>296.0476989746094</v>
       </c>
       <c r="C27">
-        <v>417.9641723632812</v>
+        <v>277.2492980957031</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -682,10 +682,10 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>382.6108093261719</v>
+        <v>293.8583068847656</v>
       </c>
       <c r="C28">
-        <v>396.9380187988281</v>
+        <v>280.3315734863281</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -693,10 +693,10 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>559.327392578125</v>
+        <v>270.598388671875</v>
       </c>
       <c r="C29">
-        <v>571.0968627929688</v>
+        <v>259.9082946777344</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -704,10 +704,10 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>322.8132934570312</v>
+        <v>386.7999877929688</v>
       </c>
       <c r="C30">
-        <v>321.6759033203125</v>
+        <v>388.9661865234375</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -715,10 +715,10 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>278.6965942382812</v>
+        <v>406.9070129394531</v>
       </c>
       <c r="C31">
-        <v>267.7920837402344</v>
+        <v>398.6802062988281</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -726,10 +726,10 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>378.1527099609375</v>
+        <v>251.5711059570312</v>
       </c>
       <c r="C32">
-        <v>395.7175598144531</v>
+        <v>246.6331176757812</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -737,10 +737,10 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>403.1365051269531</v>
+        <v>444.8670043945312</v>
       </c>
       <c r="C33">
-        <v>410.0470275878906</v>
+        <v>429.2984619140625</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -748,10 +748,10 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>432.9602050781251</v>
+        <v>296.0859985351562</v>
       </c>
       <c r="C34">
-        <v>424.4057312011719</v>
+        <v>277.7231750488281</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -759,10 +759,10 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>370.5411987304688</v>
+        <v>378.1856994628907</v>
       </c>
       <c r="C35">
-        <v>374.4684143066406</v>
+        <v>396.8080139160156</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -770,10 +770,10 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>357.7934875488281</v>
+        <v>487.5723876953125</v>
       </c>
       <c r="C36">
-        <v>361.1059875488281</v>
+        <v>484.5013122558594</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -781,10 +781,10 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>428.2267150878907</v>
+        <v>290</v>
       </c>
       <c r="C37">
-        <v>425.1068725585938</v>
+        <v>282.0383605957031</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -792,10 +792,10 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>270.1676025390625</v>
+        <v>328.1419982910156</v>
       </c>
       <c r="C38">
-        <v>275.7402954101562</v>
+        <v>308.7505798339844</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -803,10 +803,10 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>244.1571960449219</v>
+        <v>525.4376831054688</v>
       </c>
       <c r="C39">
-        <v>264.8300476074219</v>
+        <v>514.758544921875</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -814,10 +814,10 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>313.9648132324219</v>
+        <v>421.6908874511718</v>
       </c>
       <c r="C40">
-        <v>316.6191101074219</v>
+        <v>417.4161682128906</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -825,10 +825,10 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>260.3168029785156</v>
+        <v>302.6816101074219</v>
       </c>
       <c r="C41">
-        <v>295.7434997558594</v>
+        <v>278.822509765625</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -836,10 +836,10 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>398.8500061035156</v>
+        <v>422.7874145507812</v>
       </c>
       <c r="C42">
-        <v>404.5084228515625</v>
+        <v>409.8128356933594</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -847,10 +847,10 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>264.7000122070312</v>
+        <v>504.4655151367188</v>
       </c>
       <c r="C43">
-        <v>279.1662902832031</v>
+        <v>501.6289978027344</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -858,10 +858,10 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>271.5343933105469</v>
+        <v>305.3857116699219</v>
       </c>
       <c r="C44">
-        <v>287.8984069824219</v>
+        <v>292.8341979980469</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -869,10 +869,10 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>421.9486999511719</v>
+        <v>518.0999755859375</v>
       </c>
       <c r="C45">
-        <v>425.5852661132812</v>
+        <v>505.5911560058594</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -880,10 +880,10 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>299.3187866210938</v>
+        <v>426.6310119628906</v>
       </c>
       <c r="C46">
-        <v>308.1272277832031</v>
+        <v>408.800537109375</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -891,10 +891,10 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>397.4255981445312</v>
+        <v>570.2941284179688</v>
       </c>
       <c r="C47">
-        <v>404.1466369628906</v>
+        <v>578.2154541015625</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -902,10 +902,10 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>446.5696105957031</v>
+        <v>568.0811157226562</v>
       </c>
       <c r="C48">
-        <v>442.8507690429688</v>
+        <v>550.5426635742188</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -913,10 +913,10 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>392.3790893554688</v>
+        <v>522.543701171875</v>
       </c>
       <c r="C49">
-        <v>395.33349609375</v>
+        <v>510.1061401367188</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -924,10 +924,10 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>427.0698852539062</v>
+        <v>399.0376892089843</v>
       </c>
       <c r="C50">
-        <v>435.4828491210938</v>
+        <v>388.4885864257812</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -935,10 +935,10 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>280.2821960449219</v>
+        <v>285.2554931640625</v>
       </c>
       <c r="C51">
-        <v>282.9089660644531</v>
+        <v>264.5940856933594</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -946,10 +946,10 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>368.5799865722656</v>
+        <v>252.6526031494141</v>
       </c>
       <c r="C52">
-        <v>375.0992736816406</v>
+        <v>247.8816986083984</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -957,10 +957,10 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>432.2200927734375</v>
+        <v>310.2349853515625</v>
       </c>
       <c r="C53">
-        <v>435.7633361816406</v>
+        <v>300.4280700683594</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -968,10 +968,10 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>346.0790100097656</v>
+        <v>419.3989868164062</v>
       </c>
       <c r="C54">
-        <v>356.3782653808594</v>
+        <v>418.6924743652344</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -979,10 +979,10 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>413.0799865722656</v>
+        <v>586.21728515625</v>
       </c>
       <c r="C55">
-        <v>415.54541015625</v>
+        <v>576.5828247070312</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -990,10 +990,10 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>403.2296142578125</v>
+        <v>461.0997009277344</v>
       </c>
       <c r="C56">
-        <v>405.6258544921875</v>
+        <v>445.1742553710938</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1001,10 +1001,10 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>419.8310852050781</v>
+        <v>270.1676025390625</v>
       </c>
       <c r="C57">
-        <v>420.794921875</v>
+        <v>252.0648345947266</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1012,10 +1012,10 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>385.60009765625</v>
+        <v>582.8463745117188</v>
       </c>
       <c r="C58">
-        <v>411.8971252441406</v>
+        <v>573.1638793945312</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1023,10 +1023,10 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>507</v>
+        <v>419.4941101074219</v>
       </c>
       <c r="C59">
-        <v>499.0827941894531</v>
+        <v>406.0650939941406</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1034,10 +1034,10 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>586.8807983398438</v>
+        <v>264.7000122070312</v>
       </c>
       <c r="C60">
-        <v>568.2730712890625</v>
+        <v>252.988037109375</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1045,10 +1045,10 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>288.5451049804688</v>
+        <v>367</v>
       </c>
       <c r="C61">
-        <v>297.0246276855469</v>
+        <v>354.4915771484375</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1056,10 +1056,10 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>270.09130859375</v>
+        <v>427.8120117187499</v>
       </c>
       <c r="C62">
-        <v>271.7676086425781</v>
+        <v>420.1081237792969</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1067,10 +1067,10 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>274.0040893554688</v>
+        <v>390.8353881835938</v>
       </c>
       <c r="C63">
-        <v>289.6649475097656</v>
+        <v>388.4997253417969</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1078,10 +1078,10 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>419.7427062988281</v>
+        <v>549.8206787109375</v>
       </c>
       <c r="C64">
-        <v>433.4860229492188</v>
+        <v>526.965087890625</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1089,10 +1089,10 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>476.6423034667969</v>
+        <v>569.6843872070312</v>
       </c>
       <c r="C65">
-        <v>468.386474609375</v>
+        <v>559.8291015625</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1100,10 +1100,10 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>465.7080078125</v>
+        <v>278.6965942382812</v>
       </c>
       <c r="C66">
-        <v>452.6737365722656</v>
+        <v>250.4202575683594</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1111,10 +1111,10 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>284.7213134765625</v>
+        <v>260.1300048828125</v>
       </c>
       <c r="C67">
-        <v>289.8526306152344</v>
+        <v>265.61572265625</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1122,10 +1122,10 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>293.035400390625</v>
+        <v>479.9277038574219</v>
       </c>
       <c r="C68">
-        <v>296.7052001953125</v>
+        <v>529.3800048828125</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1133,10 +1133,10 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>418.4486999511719</v>
+        <v>289.2994995117188</v>
       </c>
       <c r="C69">
-        <v>412.9845886230469</v>
+        <v>266.689697265625</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1144,10 +1144,10 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>584.0484008789062</v>
+        <v>314.5404052734375</v>
       </c>
       <c r="C70">
-        <v>559.1505737304688</v>
+        <v>303.7440185546875</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1155,10 +1155,10 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>368.6400146484375</v>
+        <v>392.7562866210938</v>
       </c>
       <c r="C71">
-        <v>369.3837280273438</v>
+        <v>390.3585815429688</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1166,10 +1166,10 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>328.1419982910156</v>
+        <v>496.8670043945313</v>
       </c>
       <c r="C72">
-        <v>331.8697509765625</v>
+        <v>480.3228149414062</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1177,10 +1177,10 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>308.4100036621094</v>
+        <v>388.3716125488281</v>
       </c>
       <c r="C73">
-        <v>306.065185546875</v>
+        <v>379.7085266113281</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1188,10 +1188,10 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>401.9672851562499</v>
+        <v>420.4154052734375</v>
       </c>
       <c r="C74">
-        <v>403.9795227050781</v>
+        <v>420.4524230957031</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1199,10 +1199,10 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>495.5031127929687</v>
+        <v>421.0145874023437</v>
       </c>
       <c r="C75">
-        <v>494.7955017089844</v>
+        <v>397.7059631347656</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1210,10 +1210,10 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>498.7511901855469</v>
+        <v>398.35888671875</v>
       </c>
       <c r="C76">
-        <v>505.6542663574219</v>
+        <v>395.2691955566406</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1221,10 +1221,10 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>251.5711059570312</v>
+        <v>535.2138061523438</v>
       </c>
       <c r="C77">
-        <v>265.9999389648438</v>
+        <v>532.998779296875</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1232,10 +1232,10 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>412.3078002929688</v>
+        <v>538.1837158203125</v>
       </c>
       <c r="C78">
-        <v>431.4322204589844</v>
+        <v>537.2006225585938</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1243,10 +1243,10 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>417.9028015136719</v>
+        <v>566.7838745117188</v>
       </c>
       <c r="C79">
-        <v>416.1198120117188</v>
+        <v>553.6630249023438</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1254,10 +1254,10 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>593.3966064453125</v>
+        <v>270.9587097167969</v>
       </c>
       <c r="C80">
-        <v>573.9149169921875</v>
+        <v>248.9281311035156</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1265,10 +1265,10 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>403.4708862304688</v>
+        <v>357.7934875488281</v>
       </c>
       <c r="C81">
-        <v>396.6492919921875</v>
+        <v>350.4568786621094</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1276,10 +1276,10 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>392.4024963378906</v>
+        <v>381.3393859863281</v>
       </c>
       <c r="C82">
-        <v>408.1127014160156</v>
+        <v>376.1572265625</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1287,10 +1287,10 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>587.6348266601562</v>
+        <v>313.9648132324219</v>
       </c>
       <c r="C83">
-        <v>561.0866088867188</v>
+        <v>292.5037231445312</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1298,10 +1298,10 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>386.4367065429688</v>
+        <v>394.7203063964843</v>
       </c>
       <c r="C84">
-        <v>403.9286499023438</v>
+        <v>388.1503295898438</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1309,10 +1309,10 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>290</v>
+        <v>261.2950134277344</v>
       </c>
       <c r="C85">
-        <v>302.0779113769531</v>
+        <v>251.7735443115234</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1320,10 +1320,10 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>395.764892578125</v>
+        <v>290.0057983398438</v>
       </c>
       <c r="C86">
-        <v>401.4750061035156</v>
+        <v>265.2239990234375</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1331,10 +1331,10 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>482.893798828125</v>
+        <v>400.97509765625</v>
       </c>
       <c r="C87">
-        <v>473.6336059570312</v>
+        <v>397.9215087890625</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1342,10 +1342,10 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>395.5606994628907</v>
+        <v>424.197509765625</v>
       </c>
       <c r="C88">
-        <v>416.1013488769531</v>
+        <v>413.4684753417969</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1353,10 +1353,10 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>475.7236938476563</v>
+        <v>349.3572082519531</v>
       </c>
       <c r="C89">
-        <v>470.4190979003906</v>
+        <v>335.8493041992188</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1364,10 +1364,10 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>429.614501953125</v>
+        <v>305.4885864257812</v>
       </c>
       <c r="C90">
-        <v>419.4593200683594</v>
+        <v>298.4505310058594</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1375,10 +1375,10 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>436.4577026367188</v>
+        <v>308.4075927734375</v>
       </c>
       <c r="C91">
-        <v>439.0719909667969</v>
+        <v>288.2283325195312</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1386,10 +1386,10 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>383.6954040527344</v>
+        <v>521.1304931640625</v>
       </c>
       <c r="C92">
-        <v>398.3178405761719</v>
+        <v>503.7336730957031</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1397,10 +1397,10 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>229.1065063476562</v>
+        <v>271.5343933105469</v>
       </c>
       <c r="C93">
-        <v>277.2874450683594</v>
+        <v>269.2576293945312</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1408,10 +1408,10 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>392.2396850585937</v>
+        <v>487.1041870117188</v>
       </c>
       <c r="C94">
-        <v>405.0007629394531</v>
+        <v>466.3694152832031</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1419,10 +1419,10 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>405.8055114746094</v>
+        <v>417.910888671875</v>
       </c>
       <c r="C95">
-        <v>398.1528015136719</v>
+        <v>409.8713684082031</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1430,10 +1430,10 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>434.5</v>
+        <v>492.3669128417969</v>
       </c>
       <c r="C96">
-        <v>426.6472473144531</v>
+        <v>478.4371948242188</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1441,10 +1441,10 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>461.0997009277344</v>
+        <v>246.5</v>
       </c>
       <c r="C97">
-        <v>451.6669616699219</v>
+        <v>246.1370849609375</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1452,10 +1452,10 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>417.9410095214844</v>
+        <v>559.327392578125</v>
       </c>
       <c r="C98">
-        <v>426.6658325195312</v>
+        <v>572.3646850585938</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1463,10 +1463,10 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>396.652099609375</v>
+        <v>368.5799865722656</v>
       </c>
       <c r="C99">
-        <v>403.1630554199219</v>
+        <v>364.7281799316406</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1474,10 +1474,10 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>318.3608093261719</v>
+        <v>423.3670959472657</v>
       </c>
       <c r="C100">
-        <v>307.0036315917969</v>
+        <v>404.6732788085938</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1485,10 +1485,10 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>451.8669128417969</v>
+        <v>591.4080200195312</v>
       </c>
       <c r="C101">
-        <v>444.6144104003906</v>
+        <v>578.3184814453125</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -1496,10 +1496,10 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>404.4645080566406</v>
+        <v>270.09130859375</v>
       </c>
       <c r="C102">
-        <v>399.6914367675781</v>
+        <v>251.2371826171875</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -1507,10 +1507,10 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>304.0474853515625</v>
+        <v>421.5596923828125</v>
       </c>
       <c r="C103">
-        <v>306.7532958984375</v>
+        <v>415.1712951660156</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -1518,10 +1518,10 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>484.1395874023438</v>
+        <v>292.2999877929688</v>
       </c>
       <c r="C104">
-        <v>510.4217529296875</v>
+        <v>262.924560546875</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -1529,10 +1529,10 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>266.2799072265625</v>
+        <v>419.3635864257812</v>
       </c>
       <c r="C105">
-        <v>265.1892395019531</v>
+        <v>410.9981079101562</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -1540,10 +1540,10 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>390.8353881835938</v>
+        <v>559.3516845703125</v>
       </c>
       <c r="C106">
-        <v>395.612548828125</v>
+        <v>539.8766479492188</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -1551,10 +1551,10 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>388.7840881347656</v>
+        <v>302.9296875</v>
       </c>
       <c r="C107">
-        <v>393.3342895507812</v>
+        <v>288.6112670898438</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -1562,10 +1562,10 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>300.8251037597656</v>
+        <v>448.3281860351562</v>
       </c>
       <c r="C108">
-        <v>303.4838562011719</v>
+        <v>441.5487976074219</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -1573,10 +1573,10 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>371.0592956542969</v>
+        <v>419.847900390625</v>
       </c>
       <c r="C109">
-        <v>374.806640625</v>
+        <v>412.4140625</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -1584,10 +1584,10 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>306.07958984375</v>
+        <v>322.1997985839844</v>
       </c>
       <c r="C110">
-        <v>313.542236328125</v>
+        <v>306.5157470703125</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -1595,10 +1595,10 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>381.3393859863281</v>
+        <v>348.1325073242188</v>
       </c>
       <c r="C111">
-        <v>388.8533325195312</v>
+        <v>331.7647399902344</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -1606,10 +1606,10 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>327.5273132324219</v>
+        <v>562.5999145507812</v>
       </c>
       <c r="C112">
-        <v>332.2026062011719</v>
+        <v>557.7393188476562</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -1617,10 +1617,10 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>391.1155090332031</v>
+        <v>304.4100036621094</v>
       </c>
       <c r="C113">
-        <v>392.3465576171875</v>
+        <v>291.5958557128906</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -1628,10 +1628,10 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>434.7648925781251</v>
+        <v>308.4100036621094</v>
       </c>
       <c r="C114">
-        <v>425.5917358398438</v>
+        <v>285.658447265625</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -1639,10 +1639,10 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>328.3931884765625</v>
+        <v>401.4468078613282</v>
       </c>
       <c r="C115">
-        <v>331.1983337402344</v>
+        <v>393.2323608398438</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -1650,10 +1650,10 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>341.0456848144531</v>
+        <v>523.1370239257812</v>
       </c>
       <c r="C116">
-        <v>357.472900390625</v>
+        <v>518.0225219726562</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -1661,10 +1661,10 @@
         <v>115</v>
       </c>
       <c r="B117">
-        <v>377.414794921875</v>
+        <v>306.9997863769531</v>
       </c>
       <c r="C117">
-        <v>386.5863952636719</v>
+        <v>287.365966796875</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -1672,10 +1672,10 @@
         <v>116</v>
       </c>
       <c r="B118">
-        <v>287.9706115722656</v>
+        <v>322.7486877441406</v>
       </c>
       <c r="C118">
-        <v>283.8221130371094</v>
+        <v>288.5983276367188</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -1683,10 +1683,10 @@
         <v>117</v>
       </c>
       <c r="B119">
-        <v>316.6575012207031</v>
+        <v>294.6500854492188</v>
       </c>
       <c r="C119">
-        <v>329.4533386230469</v>
+        <v>302.0364685058594</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -1697,7 +1697,7 @@
         <v>282.5306091308594</v>
       </c>
       <c r="C120">
-        <v>274.7335205078125</v>
+        <v>261.6714477539062</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -1705,10 +1705,10 @@
         <v>119</v>
       </c>
       <c r="B121">
-        <v>273.8634033203125</v>
+        <v>288.1705932617188</v>
       </c>
       <c r="C121">
-        <v>268.8559265136719</v>
+        <v>256.2552795410156</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -1716,10 +1716,10 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>420.4154052734375</v>
+        <v>540.1475830078125</v>
       </c>
       <c r="C122">
-        <v>429.759765625</v>
+        <v>534.7506103515625</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -1727,10 +1727,10 @@
         <v>121</v>
       </c>
       <c r="B123">
-        <v>240.6813049316406</v>
+        <v>278.8116149902344</v>
       </c>
       <c r="C123">
-        <v>287.7169799804688</v>
+        <v>256.4315185546875</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -1738,10 +1738,10 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>332.5303955078125</v>
+        <v>311.7226867675781</v>
       </c>
       <c r="C124">
-        <v>334.2992248535156</v>
+        <v>288.1817932128906</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -1749,10 +1749,10 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>269.3215026855469</v>
+        <v>277.8193969726562</v>
       </c>
       <c r="C125">
-        <v>268.6250915527344</v>
+        <v>251.4733428955078</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -1760,10 +1760,10 @@
         <v>124</v>
       </c>
       <c r="B126">
-        <v>403.6130981445312</v>
+        <v>309.3153991699219</v>
       </c>
       <c r="C126">
-        <v>400.01025390625</v>
+        <v>289.0890808105469</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -1771,10 +1771,10 @@
         <v>125</v>
       </c>
       <c r="B127">
-        <v>295.0502014160156</v>
+        <v>407.5502014160156</v>
       </c>
       <c r="C127">
-        <v>285.212646484375</v>
+        <v>411.4904174804688</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -1782,10 +1782,10 @@
         <v>126</v>
       </c>
       <c r="B128">
-        <v>486.9659118652344</v>
+        <v>393.5574035644531</v>
       </c>
       <c r="C128">
-        <v>471.8625183105469</v>
+        <v>398.0490112304688</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -1793,10 +1793,10 @@
         <v>127</v>
       </c>
       <c r="B129">
-        <v>294.3194885253906</v>
+        <v>296.139892578125</v>
       </c>
       <c r="C129">
-        <v>289.51220703125</v>
+        <v>283.1841735839844</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -1804,10 +1804,10 @@
         <v>128</v>
       </c>
       <c r="B130">
-        <v>546.2999267578125</v>
+        <v>556.5263061523438</v>
       </c>
       <c r="C130">
-        <v>544.4596557617188</v>
+        <v>536.2527465820312</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -1815,10 +1815,10 @@
         <v>129</v>
       </c>
       <c r="B131">
-        <v>418.9497070312499</v>
+        <v>371.7095031738281</v>
       </c>
       <c r="C131">
-        <v>426.1278991699219</v>
+        <v>363.2998657226562</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -1826,10 +1826,10 @@
         <v>130</v>
       </c>
       <c r="B132">
-        <v>292.2301025390625</v>
+        <v>365.0610046386719</v>
       </c>
       <c r="C132">
-        <v>304.0402526855469</v>
+        <v>354.9055786132812</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -1837,10 +1837,10 @@
         <v>131</v>
       </c>
       <c r="B133">
-        <v>384.7600097656251</v>
+        <v>390.41650390625</v>
       </c>
       <c r="C133">
-        <v>386.6803283691406</v>
+        <v>403.9290771484375</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -1848,10 +1848,10 @@
         <v>132</v>
       </c>
       <c r="B134">
-        <v>280.3630065917969</v>
+        <v>326.1506042480469</v>
       </c>
       <c r="C134">
-        <v>283.857421875</v>
+        <v>306.8634643554688</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -1859,10 +1859,10 @@
         <v>133</v>
       </c>
       <c r="B135">
-        <v>290.6365051269531</v>
+        <v>244.1571960449219</v>
       </c>
       <c r="C135">
-        <v>289.3638610839844</v>
+        <v>245.7291870117188</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -1870,10 +1870,10 @@
         <v>134</v>
       </c>
       <c r="B136">
-        <v>550.5505981445312</v>
+        <v>537.1049194335938</v>
       </c>
       <c r="C136">
-        <v>532.2608642578125</v>
+        <v>537.7274780273438</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -1881,10 +1881,10 @@
         <v>135</v>
       </c>
       <c r="B137">
-        <v>475.8749084472656</v>
+        <v>412.4996032714844</v>
       </c>
       <c r="C137">
-        <v>467.8050231933594</v>
+        <v>403.6775817871094</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -1892,10 +1892,10 @@
         <v>136</v>
       </c>
       <c r="B138">
-        <v>253.4152069091797</v>
+        <v>425.7432861328124</v>
       </c>
       <c r="C138">
-        <v>266.8958129882812</v>
+        <v>429.84765625</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -1903,10 +1903,10 @@
         <v>137</v>
       </c>
       <c r="B139">
-        <v>304.2987060546875</v>
+        <v>451.8669128417969</v>
       </c>
       <c r="C139">
-        <v>315.2050170898438</v>
+        <v>437.5346069335938</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -1914,10 +1914,10 @@
         <v>138</v>
       </c>
       <c r="B140">
-        <v>512.1353759765625</v>
+        <v>383.9512939453125</v>
       </c>
       <c r="C140">
-        <v>494.901123046875</v>
+        <v>387.384033203125</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -1925,10 +1925,10 @@
         <v>139</v>
       </c>
       <c r="B141">
-        <v>259.3646850585938</v>
+        <v>322.8132934570312</v>
       </c>
       <c r="C141">
-        <v>272.2601318359375</v>
+        <v>305.6576843261719</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -1936,10 +1936,10 @@
         <v>140</v>
       </c>
       <c r="B142">
-        <v>260.4594116210938</v>
+        <v>326.1883850097656</v>
       </c>
       <c r="C142">
-        <v>278.1162109375</v>
+        <v>310.0333862304688</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -1947,10 +1947,10 @@
         <v>141</v>
       </c>
       <c r="B143">
-        <v>410.0512084960938</v>
+        <v>428.631103515625</v>
       </c>
       <c r="C143">
-        <v>408.6537170410156</v>
+        <v>427.5933532714844</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -1958,10 +1958,10 @@
         <v>142</v>
       </c>
       <c r="B144">
-        <v>303.418701171875</v>
+        <v>394.9399108886719</v>
       </c>
       <c r="C144">
-        <v>296.3648986816406</v>
+        <v>398.1915283203125</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -1969,10 +1969,10 @@
         <v>143</v>
       </c>
       <c r="B145">
-        <v>496.4932861328125</v>
+        <v>330.7618103027344</v>
       </c>
       <c r="C145">
-        <v>505.9308166503906</v>
+        <v>335.8077087402344</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -1980,10 +1980,10 @@
         <v>144</v>
       </c>
       <c r="B146">
-        <v>314.5404052734375</v>
+        <v>251.7709045410156</v>
       </c>
       <c r="C146">
-        <v>328.9762878417969</v>
+        <v>245.6165924072266</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -1991,10 +1991,10 @@
         <v>145</v>
       </c>
       <c r="B147">
-        <v>307.6572875976562</v>
+        <v>346.0790100097656</v>
       </c>
       <c r="C147">
-        <v>311.26611328125</v>
+        <v>344.683837890625</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2002,10 +2002,10 @@
         <v>146</v>
       </c>
       <c r="B148">
-        <v>331.0516967773438</v>
+        <v>436.7999877929688</v>
       </c>
       <c r="C148">
-        <v>327.3030700683594</v>
+        <v>418.7205810546875</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2013,10 +2013,10 @@
         <v>147</v>
       </c>
       <c r="B149">
-        <v>387.2174987792969</v>
+        <v>403.8982849121094</v>
       </c>
       <c r="C149">
-        <v>396.2979125976562</v>
+        <v>395.2512512207031</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2024,10 +2024,10 @@
         <v>148</v>
       </c>
       <c r="B150">
-        <v>287.330810546875</v>
+        <v>401.5698852539062</v>
       </c>
       <c r="C150">
-        <v>285.7471923828125</v>
+        <v>402.1190185546875</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2035,10 +2035,10 @@
         <v>149</v>
       </c>
       <c r="B151">
-        <v>295.5263977050781</v>
+        <v>277.6722106933594</v>
       </c>
       <c r="C151">
-        <v>320.4238891601562</v>
+        <v>255.7232360839844</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2046,10 +2046,10 @@
         <v>150</v>
       </c>
       <c r="B152">
-        <v>398.9317932128907</v>
+        <v>240.6813049316406</v>
       </c>
       <c r="C152">
-        <v>398.7120056152344</v>
+        <v>265.3895874023438</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2057,10 +2057,10 @@
         <v>151</v>
       </c>
       <c r="B153">
-        <v>255.9281005859375</v>
+        <v>241.7299957275391</v>
       </c>
       <c r="C153">
-        <v>267.5767211914062</v>
+        <v>244.4187622070312</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2068,10 +2068,10 @@
         <v>152</v>
       </c>
       <c r="B154">
-        <v>498.7596130371094</v>
+        <v>522.5180053710938</v>
       </c>
       <c r="C154">
-        <v>479.8067932128906</v>
+        <v>515.4053344726562</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2079,10 +2079,10 @@
         <v>153</v>
       </c>
       <c r="B155">
-        <v>383.9866027832032</v>
+        <v>390.7073059082032</v>
       </c>
       <c r="C155">
-        <v>406.7164916992188</v>
+        <v>392.5921020507812</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2090,10 +2090,10 @@
         <v>154</v>
       </c>
       <c r="B156">
-        <v>497.3724060058594</v>
+        <v>269.3215026855469</v>
       </c>
       <c r="C156">
-        <v>488.0827941894531</v>
+        <v>248.0434417724609</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2101,10 +2101,10 @@
         <v>155</v>
       </c>
       <c r="B157">
-        <v>588.3859252929688</v>
+        <v>280.9642944335938</v>
       </c>
       <c r="C157">
-        <v>571.91162109375</v>
+        <v>269.63623046875</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2112,10 +2112,10 @@
         <v>156</v>
       </c>
       <c r="B158">
-        <v>306.9997863769531</v>
+        <v>403.7907104492188</v>
       </c>
       <c r="C158">
-        <v>312.4679260253906</v>
+        <v>391.0464172363281</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2123,10 +2123,10 @@
         <v>157</v>
       </c>
       <c r="B159">
-        <v>404.7716979980469</v>
+        <v>538.4003295898438</v>
       </c>
       <c r="C159">
-        <v>416.0510559082031</v>
+        <v>544.4661254882812</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2134,10 +2134,10 @@
         <v>158</v>
       </c>
       <c r="B160">
-        <v>339.4797058105469</v>
+        <v>287.9706115722656</v>
       </c>
       <c r="C160">
-        <v>350.2800903320312</v>
+        <v>268.1317138671875</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2145,10 +2145,10 @@
         <v>159</v>
       </c>
       <c r="B161">
-        <v>269.0469055175781</v>
+        <v>506.2308044433594</v>
       </c>
       <c r="C161">
-        <v>275.6485290527344</v>
+        <v>499.3150634765625</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2156,10 +2156,10 @@
         <v>160</v>
       </c>
       <c r="B162">
-        <v>393.5574035644531</v>
+        <v>429.8890075683594</v>
       </c>
       <c r="C162">
-        <v>408.457275390625</v>
+        <v>424.5675048828125</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2167,10 +2167,10 @@
         <v>161</v>
       </c>
       <c r="B163">
-        <v>466.4325866699219</v>
+        <v>402.9413146972656</v>
       </c>
       <c r="C163">
-        <v>539.6298217773438</v>
+        <v>399.1835327148438</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -2178,10 +2178,10 @@
         <v>162</v>
       </c>
       <c r="B164">
-        <v>285.2554931640625</v>
+        <v>419.9999999999999</v>
       </c>
       <c r="C164">
-        <v>281.9640808105469</v>
+        <v>414.2544250488281</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -2189,10 +2189,10 @@
         <v>163</v>
       </c>
       <c r="B165">
-        <v>507.1431884765625</v>
+        <v>396.2138977050781</v>
       </c>
       <c r="C165">
-        <v>516.1868286132812</v>
+        <v>386.4717712402344</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -2200,10 +2200,10 @@
         <v>164</v>
       </c>
       <c r="B166">
-        <v>420.8039855957031</v>
+        <v>304.3093872070312</v>
       </c>
       <c r="C166">
-        <v>429.3793029785156</v>
+        <v>284.7326965332031</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -2211,10 +2211,10 @@
         <v>165</v>
       </c>
       <c r="B167">
-        <v>256.4190063476562</v>
+        <v>293.035400390625</v>
       </c>
       <c r="C167">
-        <v>268.3616943359375</v>
+        <v>271.7813110351562</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -2222,10 +2222,10 @@
         <v>166</v>
       </c>
       <c r="B168">
-        <v>348.1325073242188</v>
+        <v>547.8563842773438</v>
       </c>
       <c r="C168">
-        <v>342.4039001464844</v>
+        <v>523.51806640625</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -2233,10 +2233,10 @@
         <v>167</v>
       </c>
       <c r="B169">
-        <v>420.2900085449219</v>
+        <v>418.9497070312499</v>
       </c>
       <c r="C169">
-        <v>434.2857666015625</v>
+        <v>416.1486511230469</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -2244,10 +2244,10 @@
         <v>168</v>
       </c>
       <c r="B170">
-        <v>288.5866088867188</v>
+        <v>253.4152069091797</v>
       </c>
       <c r="C170">
-        <v>296.8683471679688</v>
+        <v>248.1417694091797</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -2255,10 +2255,10 @@
         <v>169</v>
       </c>
       <c r="B171">
-        <v>324.752197265625</v>
+        <v>403.5846862792969</v>
       </c>
       <c r="C171">
-        <v>317.2054443359375</v>
+        <v>410.3525390625</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -2266,10 +2266,10 @@
         <v>170</v>
       </c>
       <c r="B172">
-        <v>267.9208068847656</v>
+        <v>326.5101013183594</v>
       </c>
       <c r="C172">
-        <v>271.7098999023438</v>
+        <v>311.860595703125</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -2277,10 +2277,10 @@
         <v>171</v>
       </c>
       <c r="B173">
-        <v>421.5596923828125</v>
+        <v>317.8067016601562</v>
       </c>
       <c r="C173">
-        <v>425.2037048339844</v>
+        <v>320.2467956542969</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -2288,10 +2288,10 @@
         <v>172</v>
       </c>
       <c r="B174">
-        <v>270.9587097167969</v>
+        <v>259.3646850585938</v>
       </c>
       <c r="C174">
-        <v>266.9075012207031</v>
+        <v>250.5768127441406</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -2299,10 +2299,10 @@
         <v>173</v>
       </c>
       <c r="B175">
-        <v>322.1997985839844</v>
+        <v>391.1155090332031</v>
       </c>
       <c r="C175">
-        <v>327.4732360839844</v>
+        <v>379.5552368164062</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -2310,10 +2310,10 @@
         <v>174</v>
       </c>
       <c r="B176">
-        <v>402.6943054199219</v>
+        <v>260.4594116210938</v>
       </c>
       <c r="C176">
-        <v>411.3968811035156</v>
+        <v>253.0650634765625</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -2321,10 +2321,10 @@
         <v>175</v>
       </c>
       <c r="B177">
-        <v>584.731201171875</v>
+        <v>267.3150939941406</v>
       </c>
       <c r="C177">
-        <v>567.6869506835938</v>
+        <v>248.9644927978516</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -2332,10 +2332,10 @@
         <v>176</v>
       </c>
       <c r="B178">
-        <v>274.6285095214844</v>
+        <v>406.2774963378906</v>
       </c>
       <c r="C178">
-        <v>272.6240539550781</v>
+        <v>411.0078125</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -2343,10 +2343,10 @@
         <v>177</v>
       </c>
       <c r="B179">
-        <v>372.9309997558594</v>
+        <v>390.0151977539063</v>
       </c>
       <c r="C179">
-        <v>379.0478210449219</v>
+        <v>382.4635620117188</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -2354,10 +2354,10 @@
         <v>178</v>
       </c>
       <c r="B180">
-        <v>560.6566162109375</v>
+        <v>573.035888671875</v>
       </c>
       <c r="C180">
-        <v>547.5355834960938</v>
+        <v>555.8905029296875</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -2365,10 +2365,10 @@
         <v>179</v>
       </c>
       <c r="B181">
-        <v>472.0051879882812</v>
+        <v>400.76611328125</v>
       </c>
       <c r="C181">
-        <v>462.5169677734375</v>
+        <v>398.3782043457031</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -2376,10 +2376,10 @@
         <v>180</v>
       </c>
       <c r="B182">
-        <v>268.8121948242188</v>
+        <v>377.2589111328125</v>
       </c>
       <c r="C182">
-        <v>277.288818359375</v>
+        <v>369.4013061523438</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -2387,10 +2387,10 @@
         <v>181</v>
       </c>
       <c r="B183">
-        <v>392.2799987792969</v>
+        <v>392.6817932128906</v>
       </c>
       <c r="C183">
-        <v>405.6535034179688</v>
+        <v>390.5142211914062</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -2398,10 +2398,10 @@
         <v>182</v>
       </c>
       <c r="B184">
-        <v>294.6500854492188</v>
+        <v>500.5494079589843</v>
       </c>
       <c r="C184">
-        <v>322.7281188964844</v>
+        <v>501.8848571777344</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -2409,10 +2409,10 @@
         <v>183</v>
       </c>
       <c r="B185">
-        <v>251.7709045410156</v>
+        <v>300.4450073242188</v>
       </c>
       <c r="C185">
-        <v>265.4427185058594</v>
+        <v>266.6459350585938</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -2420,10 +2420,10 @@
         <v>184</v>
       </c>
       <c r="B186">
-        <v>293.1224975585938</v>
+        <v>291.335205078125</v>
       </c>
       <c r="C186">
-        <v>289.894287109375</v>
+        <v>259.632568359375</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -2431,10 +2431,10 @@
         <v>185</v>
       </c>
       <c r="B187">
-        <v>434.9754943847656</v>
+        <v>291.70849609375</v>
       </c>
       <c r="C187">
-        <v>427.4244995117188</v>
+        <v>274.1764526367188</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -2442,10 +2442,10 @@
         <v>186</v>
       </c>
       <c r="B188">
-        <v>387.5835876464844</v>
+        <v>328.3931884765625</v>
       </c>
       <c r="C188">
-        <v>399.8388671875</v>
+        <v>316.9889221191406</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -2453,10 +2453,10 @@
         <v>187</v>
       </c>
       <c r="B189">
-        <v>277.25</v>
+        <v>255.9281005859375</v>
       </c>
       <c r="C189">
-        <v>269.2424011230469</v>
+        <v>248.335205078125</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -2464,10 +2464,10 @@
         <v>188</v>
       </c>
       <c r="B190">
-        <v>300.4450073242188</v>
+        <v>519.1286010742188</v>
       </c>
       <c r="C190">
-        <v>281.3460998535156</v>
+        <v>502.0442810058594</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -2475,10 +2475,10 @@
         <v>189</v>
       </c>
       <c r="B191">
-        <v>398.5889892578125</v>
+        <v>396.69580078125</v>
       </c>
       <c r="C191">
-        <v>406.5752563476562</v>
+        <v>392.2306823730469</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -2486,10 +2486,10 @@
         <v>190</v>
       </c>
       <c r="B192">
-        <v>591.6759033203125</v>
+        <v>394.3688049316406</v>
       </c>
       <c r="C192">
-        <v>573.0191040039062</v>
+        <v>384.0310974121094</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -2497,10 +2497,10 @@
         <v>191</v>
       </c>
       <c r="B193">
-        <v>267.5842895507812</v>
+        <v>408.119384765625</v>
       </c>
       <c r="C193">
-        <v>270.3271484375</v>
+        <v>404.2712097167969</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -2508,10 +2508,10 @@
         <v>192</v>
       </c>
       <c r="B194">
-        <v>526.2675170898438</v>
+        <v>302.8817138671875</v>
       </c>
       <c r="C194">
-        <v>519.3887939453125</v>
+        <v>286.015380859375</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -2519,10 +2519,10 @@
         <v>193</v>
       </c>
       <c r="B195">
-        <v>389.2496948242188</v>
+        <v>398.6109008789062</v>
       </c>
       <c r="C195">
-        <v>400.1048278808594</v>
+        <v>393.7181396484375</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -2530,10 +2530,10 @@
         <v>194</v>
       </c>
       <c r="B196">
-        <v>393.9295043945312</v>
+        <v>418.1351928710938</v>
       </c>
       <c r="C196">
-        <v>396.8930969238281</v>
+        <v>417.9317932128906</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -2541,10 +2541,10 @@
         <v>195</v>
       </c>
       <c r="B197">
-        <v>430.0299987792969</v>
+        <v>424.0140075683593</v>
       </c>
       <c r="C197">
-        <v>432.2503356933594</v>
+        <v>429.1637573242188</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -2552,10 +2552,10 @@
         <v>196</v>
       </c>
       <c r="B198">
-        <v>394.5595092773438</v>
+        <v>571.8140258789062</v>
       </c>
       <c r="C198">
-        <v>397.6973876953125</v>
+        <v>553.713623046875</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -2563,10 +2563,10 @@
         <v>197</v>
       </c>
       <c r="B199">
-        <v>273.6575012207031</v>
+        <v>398.2062988281249</v>
       </c>
       <c r="C199">
-        <v>276.177978515625</v>
+        <v>388.7803649902344</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -2574,10 +2574,10 @@
         <v>198</v>
       </c>
       <c r="B200">
-        <v>400.6080017089844</v>
+        <v>274.0040893554688</v>
       </c>
       <c r="C200">
-        <v>408.792236328125</v>
+        <v>270.150146484375</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -2585,10 +2585,10 @@
         <v>199</v>
       </c>
       <c r="B201">
-        <v>303.2987976074219</v>
+        <v>411.74951171875</v>
       </c>
       <c r="C201">
-        <v>312.7433471679688</v>
+        <v>425.1728820800781</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -2596,10 +2596,10 @@
         <v>200</v>
       </c>
       <c r="B202">
-        <v>301.6788940429688</v>
+        <v>269.0469055175781</v>
       </c>
       <c r="C202">
-        <v>305.0091552734375</v>
+        <v>251.2502593994141</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -2607,10 +2607,10 @@
         <v>201</v>
       </c>
       <c r="B203">
-        <v>392.0765991210937</v>
+        <v>497.0021057128906</v>
       </c>
       <c r="C203">
-        <v>395.3723754882812</v>
+        <v>502.4931640625</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -2618,10 +2618,10 @@
         <v>202</v>
       </c>
       <c r="B204">
-        <v>296.0476989746094</v>
+        <v>422.6600036621094</v>
       </c>
       <c r="C204">
-        <v>299.7031860351562</v>
+        <v>414.8913879394531</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -2629,10 +2629,10 @@
         <v>203</v>
       </c>
       <c r="B205">
-        <v>369.7710876464844</v>
+        <v>392.3790893554688</v>
       </c>
       <c r="C205">
-        <v>381.3687133789062</v>
+        <v>385.0050354003906</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -2640,10 +2640,10 @@
         <v>204</v>
       </c>
       <c r="B206">
-        <v>489.4585876464844</v>
+        <v>576.5717163085938</v>
       </c>
       <c r="C206">
-        <v>543.5394897460938</v>
+        <v>579.0242309570312</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -2651,10 +2651,10 @@
         <v>205</v>
       </c>
       <c r="B207">
-        <v>568.2828979492188</v>
+        <v>515.3078002929688</v>
       </c>
       <c r="C207">
-        <v>558.684326171875</v>
+        <v>497.2756042480469</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -2662,10 +2662,10 @@
         <v>206</v>
       </c>
       <c r="B208">
-        <v>236.6174926757812</v>
+        <v>396.9056091308594</v>
       </c>
       <c r="C208">
-        <v>261.4053344726562</v>
+        <v>399.9266357421875</v>
       </c>
     </row>
     <row r="209" spans="1:3">
@@ -2673,10 +2673,10 @@
         <v>207</v>
       </c>
       <c r="B209">
-        <v>396.4142150878906</v>
+        <v>450.2468872070312</v>
       </c>
       <c r="C209">
-        <v>405.9140625</v>
+        <v>432.5739440917969</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -2684,10 +2684,10 @@
         <v>208</v>
       </c>
       <c r="B210">
-        <v>498.2655944824219</v>
+        <v>472.5169067382812</v>
       </c>
       <c r="C210">
-        <v>482.4705505371094</v>
+        <v>457.8169860839844</v>
       </c>
     </row>
     <row r="211" spans="1:3">
@@ -2695,10 +2695,10 @@
         <v>209</v>
       </c>
       <c r="B211">
-        <v>395.1025085449218</v>
+        <v>256.4190063476562</v>
       </c>
       <c r="C211">
-        <v>406.3606567382812</v>
+        <v>247.7199401855469</v>
       </c>
     </row>
     <row r="212" spans="1:3">
@@ -2706,10 +2706,10 @@
         <v>210</v>
       </c>
       <c r="B212">
-        <v>302.9296875</v>
+        <v>517.2160034179688</v>
       </c>
       <c r="C212">
-        <v>314.8107299804688</v>
+        <v>509.0578308105469</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -2717,10 +2717,10 @@
         <v>211</v>
       </c>
       <c r="B213">
-        <v>290.0057983398438</v>
+        <v>287.5</v>
       </c>
       <c r="C213">
-        <v>279.0191955566406</v>
+        <v>256.6576843261719</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -2728,10 +2728,10 @@
         <v>212</v>
       </c>
       <c r="B214">
-        <v>369.81298828125</v>
+        <v>434.5</v>
       </c>
       <c r="C214">
-        <v>396.5481872558594</v>
+        <v>418.9132690429688</v>
       </c>
     </row>
     <row r="215" spans="1:3">
@@ -2739,10 +2739,10 @@
         <v>213</v>
       </c>
       <c r="B215">
-        <v>592.144775390625</v>
+        <v>496.610107421875</v>
       </c>
       <c r="C215">
-        <v>568.4224243164062</v>
+        <v>508.8388977050781</v>
       </c>
     </row>
     <row r="216" spans="1:3">
@@ -2753,7 +2753,7 @@
         <v>310.7449951171875</v>
       </c>
       <c r="C216">
-        <v>311.4411010742188</v>
+        <v>287.9163818359375</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -2761,10 +2761,10 @@
         <v>215</v>
       </c>
       <c r="B217">
-        <v>296.0950927734375</v>
+        <v>422.9324951171874</v>
       </c>
       <c r="C217">
-        <v>299.4062194824219</v>
+        <v>421.16552734375</v>
       </c>
     </row>
     <row r="218" spans="1:3">
@@ -2772,10 +2772,10 @@
         <v>216</v>
       </c>
       <c r="B218">
-        <v>292.4132995605469</v>
+        <v>267.9208068847656</v>
       </c>
       <c r="C218">
-        <v>291.0840454101562</v>
+        <v>251.5844879150391</v>
       </c>
     </row>
     <row r="219" spans="1:3">
@@ -2783,10 +2783,10 @@
         <v>217</v>
       </c>
       <c r="B219">
-        <v>398.1098937988281</v>
+        <v>425.4769897460937</v>
       </c>
       <c r="C219">
-        <v>407.6680908203125</v>
+        <v>415.7840881347656</v>
       </c>
     </row>
     <row r="220" spans="1:3">
@@ -2794,10 +2794,10 @@
         <v>218</v>
       </c>
       <c r="B220">
-        <v>297.0780029296875</v>
+        <v>502.5419006347656</v>
       </c>
       <c r="C220">
-        <v>300.7373352050781</v>
+        <v>520.0914916992188</v>
       </c>
     </row>
     <row r="221" spans="1:3">
@@ -2805,10 +2805,10 @@
         <v>219</v>
       </c>
       <c r="B221">
-        <v>330.9771118164062</v>
+        <v>295.1799926757812</v>
       </c>
       <c r="C221">
-        <v>323.6278686523438</v>
+        <v>275.305908203125</v>
       </c>
     </row>
     <row r="222" spans="1:3">
@@ -2816,10 +2816,10 @@
         <v>220</v>
       </c>
       <c r="B222">
-        <v>513.981689453125</v>
+        <v>400.764404296875</v>
       </c>
       <c r="C222">
-        <v>492.5418090820312</v>
+        <v>388.6783752441406</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -2827,10 +2827,10 @@
         <v>221</v>
       </c>
       <c r="B223">
-        <v>527.985595703125</v>
+        <v>520.8344116210938</v>
       </c>
       <c r="C223">
-        <v>516.3577880859375</v>
+        <v>516.796875</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -2838,10 +2838,10 @@
         <v>222</v>
       </c>
       <c r="B224">
-        <v>396.2138977050781</v>
+        <v>398.7380981445312</v>
       </c>
       <c r="C224">
-        <v>394.7991943359375</v>
+        <v>395.7536010742188</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -2849,10 +2849,10 @@
         <v>223</v>
       </c>
       <c r="B225">
-        <v>582.8463745117188</v>
+        <v>543.6516723632812</v>
       </c>
       <c r="C225">
-        <v>564.7412719726562</v>
+        <v>546.0910034179688</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -2860,10 +2860,10 @@
         <v>224</v>
       </c>
       <c r="B226">
-        <v>429.1943054199219</v>
+        <v>549.1870727539062</v>
       </c>
       <c r="C226">
-        <v>420.052001953125</v>
+        <v>551.2741088867188</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -2871,10 +2871,10 @@
         <v>225</v>
       </c>
       <c r="B227">
-        <v>289.2994995117188</v>
+        <v>307.8164978027344</v>
       </c>
       <c r="C227">
-        <v>289.3352966308594</v>
+        <v>289.0550537109375</v>
       </c>
     </row>
     <row r="228" spans="1:3">
@@ -2882,10 +2882,10 @@
         <v>226</v>
       </c>
       <c r="B228">
-        <v>305.5209045410156</v>
+        <v>419.5296936035156</v>
       </c>
       <c r="C228">
-        <v>323.1451721191406</v>
+        <v>409.0169677734375</v>
       </c>
     </row>
     <row r="229" spans="1:3">
@@ -2893,10 +2893,10 @@
         <v>227</v>
       </c>
       <c r="B229">
-        <v>399.330810546875</v>
+        <v>268.8121948242188</v>
       </c>
       <c r="C229">
-        <v>398.3543395996094</v>
+        <v>254.6029968261719</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -2904,10 +2904,10 @@
         <v>228</v>
       </c>
       <c r="B230">
-        <v>449.7156982421875</v>
+        <v>472.9313049316406</v>
       </c>
       <c r="C230">
-        <v>451.3560791015625</v>
+        <v>548.0889282226562</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -2915,10 +2915,10 @@
         <v>229</v>
       </c>
       <c r="B231">
-        <v>257.698486328125</v>
+        <v>404.4645080566406</v>
       </c>
       <c r="C231">
-        <v>280.7986755371094</v>
+        <v>391.1940002441406</v>
       </c>
     </row>
     <row r="232" spans="1:3">
@@ -2926,10 +2926,10 @@
         <v>230</v>
       </c>
       <c r="B232">
-        <v>398.1430969238281</v>
+        <v>428.3505859375</v>
       </c>
       <c r="C232">
-        <v>406.9105834960938</v>
+        <v>425.0322265625</v>
       </c>
     </row>
     <row r="233" spans="1:3">
@@ -2937,10 +2937,10 @@
         <v>231</v>
       </c>
       <c r="B233">
-        <v>540.7274780273438</v>
+        <v>395.1661071777344</v>
       </c>
       <c r="C233">
-        <v>540.7028198242188</v>
+        <v>386.7929077148438</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -2948,10 +2948,10 @@
         <v>232</v>
       </c>
       <c r="B234">
-        <v>241.7299957275391</v>
+        <v>545.6931762695312</v>
       </c>
       <c r="C234">
-        <v>261.1150207519531</v>
+        <v>522.0386352539062</v>
       </c>
     </row>
     <row r="235" spans="1:3">
@@ -2959,10 +2959,10 @@
         <v>233</v>
       </c>
       <c r="B235">
-        <v>293.87890625</v>
+        <v>416.6900024414063</v>
       </c>
       <c r="C235">
-        <v>289.3816223144531</v>
+        <v>399.9214172363281</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -2970,10 +2970,10 @@
         <v>234</v>
       </c>
       <c r="B236">
-        <v>383.2698059082032</v>
+        <v>427.0698852539062</v>
       </c>
       <c r="C236">
-        <v>391.7564392089844</v>
+        <v>425.8840026855469</v>
       </c>
     </row>
     <row r="237" spans="1:3">
@@ -2981,10 +2981,10 @@
         <v>235</v>
       </c>
       <c r="B237">
-        <v>520.1492919921875</v>
+        <v>277.25</v>
       </c>
       <c r="C237">
-        <v>514.5323486328125</v>
+        <v>252.1498107910156</v>
       </c>
     </row>
     <row r="238" spans="1:3">
@@ -2992,10 +2992,10 @@
         <v>236</v>
       </c>
       <c r="B238">
-        <v>482.1986083984375</v>
+        <v>539.431884765625</v>
       </c>
       <c r="C238">
-        <v>473.0608520507812</v>
+        <v>525.6549072265625</v>
       </c>
     </row>
     <row r="239" spans="1:3">
@@ -3003,10 +3003,10 @@
         <v>237</v>
       </c>
       <c r="B239">
-        <v>394.9399108886719</v>
+        <v>401.1471862792969</v>
       </c>
       <c r="C239">
-        <v>407.9578552246094</v>
+        <v>398.2998962402344</v>
       </c>
     </row>
     <row r="240" spans="1:3">
@@ -3014,10 +3014,10 @@
         <v>238</v>
       </c>
       <c r="B240">
-        <v>302.8811950683594</v>
+        <v>401.9672851562499</v>
       </c>
       <c r="C240">
-        <v>302.3164672851562</v>
+        <v>392.5476684570312</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -3025,10 +3025,10 @@
         <v>239</v>
       </c>
       <c r="B241">
-        <v>288.1705932617188</v>
+        <v>392.0387878417968</v>
       </c>
       <c r="C241">
-        <v>272.7088317871094</v>
+        <v>389.1722106933594</v>
       </c>
     </row>
     <row r="242" spans="1:3">
@@ -3036,10 +3036,10 @@
         <v>240</v>
       </c>
       <c r="B242">
-        <v>368.6355895996094</v>
+        <v>267.5842895507812</v>
       </c>
       <c r="C242">
-        <v>372.9381408691406</v>
+        <v>249.2537841796875</v>
       </c>
     </row>
     <row r="243" spans="1:3">
@@ -3047,10 +3047,10 @@
         <v>241</v>
       </c>
       <c r="B243">
-        <v>293.0234069824219</v>
+        <v>533.7999877929688</v>
       </c>
       <c r="C243">
-        <v>291.8731384277344</v>
+        <v>543.3206787109375</v>
       </c>
     </row>
     <row r="244" spans="1:3">
@@ -3058,10 +3058,10 @@
         <v>242</v>
       </c>
       <c r="B244">
-        <v>505.0982055664062</v>
+        <v>370.4501953125</v>
       </c>
       <c r="C244">
-        <v>506.9296264648438</v>
+        <v>365.2249755859375</v>
       </c>
     </row>
     <row r="245" spans="1:3">
@@ -3069,10 +3069,10 @@
         <v>243</v>
       </c>
       <c r="B245">
-        <v>307.8164978027344</v>
+        <v>449.7156982421875</v>
       </c>
       <c r="C245">
-        <v>312.2973022460938</v>
+        <v>440.262451171875</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -3080,10 +3080,10 @@
         <v>244</v>
       </c>
       <c r="B246">
-        <v>267.3150939941406</v>
+        <v>284.7213134765625</v>
       </c>
       <c r="C246">
-        <v>266.2842102050781</v>
+        <v>274.2750549316406</v>
       </c>
     </row>
     <row r="247" spans="1:3">
@@ -3091,10 +3091,10 @@
         <v>245</v>
       </c>
       <c r="B247">
-        <v>277.8193969726562</v>
+        <v>280.2821960449219</v>
       </c>
       <c r="C247">
-        <v>269.2193298339844</v>
+        <v>264.4226379394531</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -3102,10 +3102,10 @@
         <v>246</v>
       </c>
       <c r="B248">
-        <v>506.2308044433594</v>
+        <v>405.0700073242188</v>
       </c>
       <c r="C248">
-        <v>502.4875793457031</v>
+        <v>406.0880432128906</v>
       </c>
     </row>
     <row r="249" spans="1:3">
@@ -3113,10 +3113,10 @@
         <v>247</v>
       </c>
       <c r="B249">
-        <v>280.9642944335938</v>
+        <v>392.0765991210937</v>
       </c>
       <c r="C249">
-        <v>292.4208374023438</v>
+        <v>386.2654113769531</v>
       </c>
     </row>
     <row r="250" spans="1:3">
@@ -3124,10 +3124,10 @@
         <v>248</v>
       </c>
       <c r="B250">
-        <v>388.3716125488281</v>
+        <v>287.330810546875</v>
       </c>
       <c r="C250">
-        <v>392.0330810546875</v>
+        <v>269.2750854492188</v>
       </c>
     </row>
     <row r="251" spans="1:3">
@@ -3135,10 +3135,10 @@
         <v>249</v>
       </c>
       <c r="B251">
-        <v>410.8262023925781</v>
+        <v>273.6575012207031</v>
       </c>
       <c r="C251">
-        <v>414.2388916015625</v>
+        <v>251.5146789550781</v>
       </c>
     </row>
     <row r="252" spans="1:3">
@@ -3146,10 +3146,10 @@
         <v>250</v>
       </c>
       <c r="B252">
-        <v>551.2753295898438</v>
+        <v>399.6213989257812</v>
       </c>
       <c r="C252">
-        <v>531.45703125</v>
+        <v>390.4412231445312</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -3157,10 +3157,10 @@
         <v>251</v>
       </c>
       <c r="B253">
-        <v>431.3703002929688</v>
+        <v>551.5933837890625</v>
       </c>
       <c r="C253">
-        <v>434.7646789550781</v>
+        <v>525.1854858398438</v>
       </c>
     </row>
     <row r="254" spans="1:3">
@@ -3168,10 +3168,10 @@
         <v>252</v>
       </c>
       <c r="B254">
-        <v>290.6275939941406</v>
+        <v>433.6000061035156</v>
       </c>
       <c r="C254">
-        <v>277.0893249511719</v>
+        <v>418.6626892089844</v>
       </c>
     </row>
     <row r="255" spans="1:3">
@@ -3179,10 +3179,10 @@
         <v>253</v>
       </c>
       <c r="B255">
-        <v>383.9512939453125</v>
+        <v>393.5765991210937</v>
       </c>
       <c r="C255">
-        <v>394.5947875976562</v>
+        <v>398.291259765625</v>
       </c>
     </row>
     <row r="256" spans="1:3">
@@ -3190,10 +3190,10 @@
         <v>254</v>
       </c>
       <c r="B256">
-        <v>431.6600036621094</v>
+        <v>314.0155029296875</v>
       </c>
       <c r="C256">
-        <v>428.3672790527344</v>
+        <v>302.5565185546875</v>
       </c>
     </row>
     <row r="257" spans="1:3">
@@ -3201,10 +3201,10 @@
         <v>255</v>
       </c>
       <c r="B257">
-        <v>304.3093872070312</v>
+        <v>344.9400024414062</v>
       </c>
       <c r="C257">
-        <v>309.7228698730469</v>
+        <v>336.4199829101562</v>
       </c>
     </row>
     <row r="258" spans="1:3">
@@ -3212,10 +3212,10 @@
         <v>256</v>
       </c>
       <c r="B258">
-        <v>395.7799987792969</v>
+        <v>432.0299987792969</v>
       </c>
       <c r="C258">
-        <v>409.6496887207031</v>
+        <v>416.9174194335938</v>
       </c>
     </row>
     <row r="259" spans="1:3">
@@ -3223,10 +3223,10 @@
         <v>257</v>
       </c>
       <c r="B259">
-        <v>395.2348937988281</v>
+        <v>497.3724060058594</v>
       </c>
       <c r="C259">
-        <v>395.3128662109375</v>
+        <v>483.6683959960938</v>
       </c>
     </row>
     <row r="260" spans="1:3">
@@ -3234,10 +3234,10 @@
         <v>258</v>
       </c>
       <c r="B260">
-        <v>283.5799865722656</v>
+        <v>236.6174926757812</v>
       </c>
       <c r="C260">
-        <v>277.6302490234375</v>
+        <v>244.6122131347656</v>
       </c>
     </row>
     <row r="261" spans="1:3">
@@ -3245,10 +3245,10 @@
         <v>259</v>
       </c>
       <c r="B261">
-        <v>428.4053039550781</v>
+        <v>297.0780029296875</v>
       </c>
       <c r="C261">
-        <v>424.0324096679688</v>
+        <v>278.6451416015625</v>
       </c>
     </row>
     <row r="262" spans="1:3">
@@ -3256,10 +3256,10 @@
         <v>260</v>
       </c>
       <c r="B262">
-        <v>518.0999755859375</v>
+        <v>505.6991882324219</v>
       </c>
       <c r="C262">
-        <v>507.6907653808594</v>
+        <v>501.9662170410156</v>
       </c>
     </row>
     <row r="263" spans="1:3">
@@ -3267,10 +3267,10 @@
         <v>261</v>
       </c>
       <c r="B263">
-        <v>393.4367980957032</v>
+        <v>534.836669921875</v>
       </c>
       <c r="C263">
-        <v>409.9215698242188</v>
+        <v>535.8358154296875</v>
       </c>
     </row>
     <row r="264" spans="1:3">
@@ -3278,10 +3278,10 @@
         <v>262</v>
       </c>
       <c r="B264">
-        <v>404.8301086425781</v>
+        <v>430.8338012695312</v>
       </c>
       <c r="C264">
-        <v>406.6278381347656</v>
+        <v>425.8426208496094</v>
       </c>
     </row>
     <row r="265" spans="1:3">
@@ -3289,10 +3289,10 @@
         <v>263</v>
       </c>
       <c r="B265">
-        <v>400.76611328125</v>
+        <v>389.1973876953125</v>
       </c>
       <c r="C265">
-        <v>409.2349243164062</v>
+        <v>385.9329833984375</v>
       </c>
     </row>
     <row r="266" spans="1:3">
@@ -3300,10 +3300,10 @@
         <v>264</v>
       </c>
       <c r="B266">
-        <v>488.4848937988282</v>
+        <v>304.2987060546875</v>
       </c>
       <c r="C266">
-        <v>479.4374084472656</v>
+        <v>290.1559448242188</v>
       </c>
     </row>
     <row r="267" spans="1:3">
@@ -3311,10 +3311,10 @@
         <v>265</v>
       </c>
       <c r="B267">
-        <v>260.4400024414062</v>
+        <v>539.9835815429688</v>
       </c>
       <c r="C267">
-        <v>274.1897277832031</v>
+        <v>533.946044921875</v>
       </c>
     </row>
     <row r="268" spans="1:3">
@@ -3322,10 +3322,10 @@
         <v>266</v>
       </c>
       <c r="B268">
-        <v>370.4501953125</v>
+        <v>414.1193847656251</v>
       </c>
       <c r="C268">
-        <v>375.7237854003906</v>
+        <v>415.5365905761719</v>
       </c>
     </row>
     <row r="269" spans="1:3">
@@ -3333,10 +3333,10 @@
         <v>267</v>
       </c>
       <c r="B269">
-        <v>288.1661987304688</v>
+        <v>317.3245849609375</v>
       </c>
       <c r="C269">
-        <v>294.0123901367188</v>
+        <v>301.1651306152344</v>
       </c>
     </row>
     <row r="270" spans="1:3">
@@ -3344,10 +3344,10 @@
         <v>268</v>
       </c>
       <c r="B270">
-        <v>270.2076110839844</v>
+        <v>424.9500122070312</v>
       </c>
       <c r="C270">
-        <v>268.3262634277344</v>
+        <v>430.5950622558594</v>
       </c>
     </row>
     <row r="271" spans="1:3">
@@ -3355,10 +3355,10 @@
         <v>269</v>
       </c>
       <c r="B271">
-        <v>326.5101013183594</v>
+        <v>516.5307006835938</v>
       </c>
       <c r="C271">
-        <v>333.6728515625</v>
+        <v>501.1498718261719</v>
       </c>
     </row>
     <row r="272" spans="1:3">
@@ -3366,10 +3366,10 @@
         <v>270</v>
       </c>
       <c r="B272">
-        <v>287.5</v>
+        <v>563.765625</v>
       </c>
       <c r="C272">
-        <v>272.8682556152344</v>
+        <v>560.602783203125</v>
       </c>
     </row>
     <row r="273" spans="1:3">
@@ -3377,10 +3377,10 @@
         <v>271</v>
       </c>
       <c r="B273">
-        <v>400.6438903808594</v>
+        <v>422.4660949707032</v>
       </c>
       <c r="C273">
-        <v>404.31201171875</v>
+        <v>422.3386535644531</v>
       </c>
     </row>
     <row r="274" spans="1:3">
@@ -3388,10 +3388,10 @@
         <v>272</v>
       </c>
       <c r="B274">
-        <v>475.7850036621094</v>
+        <v>307.6572875976562</v>
       </c>
       <c r="C274">
-        <v>466.7566528320312</v>
+        <v>287.3126525878906</v>
       </c>
     </row>
     <row r="275" spans="1:3">
@@ -3399,10 +3399,10 @@
         <v>273</v>
       </c>
       <c r="B275">
-        <v>317.8067016601562</v>
+        <v>257.698486328125</v>
       </c>
       <c r="C275">
-        <v>336.5036315917969</v>
+        <v>256.119873046875</v>
       </c>
     </row>
     <row r="276" spans="1:3">
@@ -3410,10 +3410,10 @@
         <v>274</v>
       </c>
       <c r="B276">
-        <v>307.4703979492188</v>
+        <v>428.0338134765624</v>
       </c>
       <c r="C276">
-        <v>316.720703125</v>
+        <v>416.9268188476562</v>
       </c>
     </row>
     <row r="277" spans="1:3">
@@ -3421,10 +3421,10 @@
         <v>275</v>
       </c>
       <c r="B277">
-        <v>317.3245849609375</v>
+        <v>304.0939025878906</v>
       </c>
       <c r="C277">
-        <v>327.5474548339844</v>
+        <v>282.1203002929688</v>
       </c>
     </row>
     <row r="278" spans="1:3">
@@ -3432,10 +3432,10 @@
         <v>276</v>
       </c>
       <c r="B278">
-        <v>386</v>
+        <v>593.1585083007812</v>
       </c>
       <c r="C278">
-        <v>401.4979553222656</v>
+        <v>580.1222534179688</v>
       </c>
     </row>
     <row r="279" spans="1:3">
@@ -3443,10 +3443,10 @@
         <v>277</v>
       </c>
       <c r="B279">
-        <v>418.510986328125</v>
+        <v>553.924072265625</v>
       </c>
       <c r="C279">
-        <v>422.5120239257812</v>
+        <v>548.9430541992188</v>
       </c>
     </row>
     <row r="280" spans="1:3">
@@ -3454,10 +3454,10 @@
         <v>278</v>
       </c>
       <c r="B280">
-        <v>400.97509765625</v>
+        <v>417.802490234375</v>
       </c>
       <c r="C280">
-        <v>409.4580078125</v>
+        <v>406.0836791992188</v>
       </c>
     </row>
     <row r="281" spans="1:3">
@@ -3465,10 +3465,10 @@
         <v>279</v>
       </c>
       <c r="B281">
-        <v>263.0103149414062</v>
+        <v>548.2901000976562</v>
       </c>
       <c r="C281">
-        <v>302.7700805664062</v>
+        <v>538.71728515625</v>
       </c>
     </row>
     <row r="282" spans="1:3">
@@ -3476,10 +3476,10 @@
         <v>280</v>
       </c>
       <c r="B282">
-        <v>275</v>
+        <v>330.9771118164062</v>
       </c>
       <c r="C282">
-        <v>267.8708190917969</v>
+        <v>311.7066040039062</v>
       </c>
     </row>
     <row r="283" spans="1:3">
@@ -3487,10 +3487,10 @@
         <v>281</v>
       </c>
       <c r="B283">
-        <v>486.2999877929688</v>
+        <v>395.5606994628907</v>
       </c>
       <c r="C283">
-        <v>481.9768371582031</v>
+        <v>406.7044372558594</v>
       </c>
     </row>
     <row r="284" spans="1:3">
@@ -3498,10 +3498,10 @@
         <v>282</v>
       </c>
       <c r="B284">
-        <v>295.5888977050781</v>
+        <v>396.75</v>
       </c>
       <c r="C284">
-        <v>289.8740844726562</v>
+        <v>389.3558044433594</v>
       </c>
     </row>
     <row r="285" spans="1:3">
@@ -3509,10 +3509,10 @@
         <v>283</v>
       </c>
       <c r="B285">
-        <v>253.0278015136719</v>
+        <v>578.4058227539062</v>
       </c>
       <c r="C285">
-        <v>265.0483093261719</v>
+        <v>563.7864990234375</v>
       </c>
     </row>
     <row r="286" spans="1:3">
@@ -3520,10 +3520,10 @@
         <v>284</v>
       </c>
       <c r="B286">
-        <v>514.4263916015625</v>
+        <v>288.5451049804688</v>
       </c>
       <c r="C286">
-        <v>518.5036010742188</v>
+        <v>274.2433471679688</v>
       </c>
     </row>
     <row r="287" spans="1:3">
@@ -3531,10 +3531,10 @@
         <v>285</v>
       </c>
       <c r="B287">
-        <v>560.519287109375</v>
+        <v>290.6365051269531</v>
       </c>
       <c r="C287">
-        <v>533.5726318359375</v>
+        <v>269.1839294433594</v>
       </c>
     </row>
     <row r="288" spans="1:3">
@@ -3542,10 +3542,10 @@
         <v>286</v>
       </c>
       <c r="B288">
-        <v>568.0811157226562</v>
+        <v>446.5696105957031</v>
       </c>
       <c r="C288">
-        <v>548.8851928710938</v>
+        <v>431.9324340820312</v>
       </c>
     </row>
     <row r="289" spans="1:3">
@@ -3553,10 +3553,10 @@
         <v>287</v>
       </c>
       <c r="B289">
-        <v>302.8817138671875</v>
+        <v>474.7710876464844</v>
       </c>
       <c r="C289">
-        <v>309.0306091308594</v>
+        <v>464.4656066894531</v>
       </c>
     </row>
     <row r="290" spans="1:3">
@@ -3564,10 +3564,10 @@
         <v>288</v>
       </c>
       <c r="B290">
-        <v>466.0299987792968</v>
+        <v>553.2366943359375</v>
       </c>
       <c r="C290">
-        <v>454.236083984375</v>
+        <v>547.2415771484375</v>
       </c>
     </row>
     <row r="291" spans="1:3">
@@ -3575,10 +3575,10 @@
         <v>289</v>
       </c>
       <c r="B291">
-        <v>593.80810546875</v>
+        <v>569.0629272460938</v>
       </c>
       <c r="C291">
-        <v>569.47412109375</v>
+        <v>553.5241088867188</v>
       </c>
     </row>
     <row r="292" spans="1:3">
@@ -3586,10 +3586,10 @@
         <v>290</v>
       </c>
       <c r="B292">
-        <v>283.4081115722656</v>
+        <v>418.510986328125</v>
       </c>
       <c r="C292">
-        <v>293.4486389160156</v>
+        <v>410.3252868652344</v>
       </c>
     </row>
     <row r="293" spans="1:3">
@@ -3597,10 +3597,10 @@
         <v>291</v>
       </c>
       <c r="B293">
-        <v>274</v>
+        <v>354.4017028808594</v>
       </c>
       <c r="C293">
-        <v>268.5757446289062</v>
+        <v>348.5312805175781</v>
       </c>
     </row>
     <row r="294" spans="1:3">
@@ -3608,10 +3608,10 @@
         <v>292</v>
       </c>
       <c r="B294">
-        <v>372.0499877929688</v>
+        <v>423.7659912109376</v>
       </c>
       <c r="C294">
-        <v>378.7800903320312</v>
+        <v>419.90185546875</v>
       </c>
     </row>
     <row r="295" spans="1:3">
@@ -3619,10 +3619,10 @@
         <v>293</v>
       </c>
       <c r="B295">
-        <v>279.0700073242188</v>
+        <v>302.6199951171875</v>
       </c>
       <c r="C295">
-        <v>286.9452209472656</v>
+        <v>292.5453796386719</v>
       </c>
     </row>
     <row r="296" spans="1:3">
@@ -3630,10 +3630,10 @@
         <v>294</v>
       </c>
       <c r="B296">
-        <v>379.9092102050781</v>
+        <v>390.6589965820312</v>
       </c>
       <c r="C296">
-        <v>389.90234375</v>
+        <v>387.288818359375</v>
       </c>
     </row>
     <row r="297" spans="1:3">
@@ -3641,10 +3641,10 @@
         <v>295</v>
       </c>
       <c r="B297">
-        <v>488.3667907714844</v>
+        <v>288.5866088867188</v>
       </c>
       <c r="C297">
-        <v>478.5460205078125</v>
+        <v>274.4061279296875</v>
       </c>
     </row>
     <row r="298" spans="1:3">
@@ -3652,10 +3652,10 @@
         <v>296</v>
       </c>
       <c r="B298">
-        <v>397.69970703125</v>
+        <v>399.5494995117188</v>
       </c>
       <c r="C298">
-        <v>403.3455200195312</v>
+        <v>414.455078125</v>
       </c>
     </row>
     <row r="299" spans="1:3">
@@ -3663,10 +3663,10 @@
         <v>297</v>
       </c>
       <c r="B299">
-        <v>302.6816101074219</v>
+        <v>283.5799865722656</v>
       </c>
       <c r="C299">
-        <v>297.5610656738281</v>
+        <v>264.2940368652344</v>
       </c>
     </row>
     <row r="300" spans="1:3">
@@ -3674,10 +3674,10 @@
         <v>298</v>
       </c>
       <c r="B300">
-        <v>398.3822937011719</v>
+        <v>548.9907836914062</v>
       </c>
       <c r="C300">
-        <v>408.8157348632812</v>
+        <v>527.5686645507812</v>
       </c>
     </row>
     <row r="301" spans="1:3">
@@ -3685,10 +3685,10 @@
         <v>299</v>
       </c>
       <c r="B301">
-        <v>364.6900024414062</v>
+        <v>263.0103149414062</v>
       </c>
       <c r="C301">
-        <v>407.2859497070312</v>
+        <v>281.4801635742188</v>
       </c>
     </row>
     <row r="302" spans="1:3">
@@ -3696,10 +3696,10 @@
         <v>300</v>
       </c>
       <c r="B302">
-        <v>591.4080200195312</v>
+        <v>421.2738037109375</v>
       </c>
       <c r="C302">
-        <v>571.7958374023438</v>
+        <v>416.1432800292969</v>
       </c>
     </row>
     <row r="303" spans="1:3">
@@ -3707,10 +3707,10 @@
         <v>301</v>
       </c>
       <c r="B303">
-        <v>417.2637023925781</v>
+        <v>425.1300048828125</v>
       </c>
       <c r="C303">
-        <v>423.2697448730469</v>
+        <v>412.3597412109375</v>
       </c>
     </row>
     <row r="304" spans="1:3">
@@ -3718,10 +3718,10 @@
         <v>302</v>
       </c>
       <c r="B304">
-        <v>288.618408203125</v>
+        <v>433.8200073242188</v>
       </c>
       <c r="C304">
-        <v>284.4250183105469</v>
+        <v>415.4201354980469</v>
       </c>
     </row>
     <row r="305" spans="1:3">
@@ -3729,10 +3729,10 @@
         <v>303</v>
       </c>
       <c r="B305">
-        <v>412.2025146484375</v>
+        <v>386.1239013671875</v>
       </c>
       <c r="C305">
-        <v>402.7657775878906</v>
+        <v>384.3160705566406</v>
       </c>
     </row>
     <row r="306" spans="1:3">
@@ -3740,10 +3740,10 @@
         <v>304</v>
       </c>
       <c r="B306">
-        <v>377.7564086914062</v>
+        <v>260.4400024414062</v>
       </c>
       <c r="C306">
-        <v>396.8580322265625</v>
+        <v>250.8175201416016</v>
       </c>
     </row>
     <row r="307" spans="1:3">
@@ -3751,10 +3751,10 @@
         <v>305</v>
       </c>
       <c r="B307">
-        <v>369.1452026367188</v>
+        <v>316.6575012207031</v>
       </c>
       <c r="C307">
-        <v>369.5752258300781</v>
+        <v>310.6487731933594</v>
       </c>
     </row>
     <row r="308" spans="1:3">
@@ -3762,10 +3762,10 @@
         <v>306</v>
       </c>
       <c r="B308">
-        <v>428.7688903808594</v>
+        <v>288.1661987304688</v>
       </c>
       <c r="C308">
-        <v>423.4382934570312</v>
+        <v>270.6522827148438</v>
       </c>
     </row>
     <row r="309" spans="1:3">
@@ -3773,10 +3773,10 @@
         <v>307</v>
       </c>
       <c r="B309">
-        <v>354.4017028808594</v>
+        <v>270.2076110839844</v>
       </c>
       <c r="C309">
-        <v>359.8312072753906</v>
+        <v>248.2527465820312</v>
       </c>
     </row>
     <row r="310" spans="1:3">
@@ -3784,10 +3784,10 @@
         <v>308</v>
       </c>
       <c r="B310">
-        <v>304.4100036621094</v>
+        <v>569.0404052734375</v>
       </c>
       <c r="C310">
-        <v>312.7871704101562</v>
+        <v>560.8665771484375</v>
       </c>
     </row>
     <row r="311" spans="1:3">
@@ -3795,10 +3795,10 @@
         <v>309</v>
       </c>
       <c r="B311">
-        <v>391.4443969726562</v>
+        <v>327.5273132324219</v>
       </c>
       <c r="C311">
-        <v>403.3112487792969</v>
+        <v>309.8790283203125</v>
       </c>
     </row>
     <row r="312" spans="1:3">
@@ -3806,10 +3806,10 @@
         <v>310</v>
       </c>
       <c r="B312">
-        <v>569.57177734375</v>
+        <v>405.5700073242188</v>
       </c>
       <c r="C312">
-        <v>572.1312255859375</v>
+        <v>403.12939453125</v>
       </c>
     </row>
     <row r="313" spans="1:3">
@@ -3817,10 +3817,10 @@
         <v>311</v>
       </c>
       <c r="B313">
-        <v>423.3670959472657</v>
+        <v>395.1025085449218</v>
       </c>
       <c r="C313">
-        <v>415.2689819335938</v>
+        <v>397.0484313964844</v>
       </c>
     </row>
     <row r="314" spans="1:3">
@@ -3828,10 +3828,10 @@
         <v>312</v>
       </c>
       <c r="B314">
-        <v>305.3857116699219</v>
+        <v>274.6285095214844</v>
       </c>
       <c r="C314">
-        <v>313.5319519042969</v>
+        <v>256.6632995605469</v>
       </c>
     </row>
     <row r="315" spans="1:3">
@@ -3839,10 +3839,10 @@
         <v>313</v>
       </c>
       <c r="B315">
-        <v>419.2052001953125</v>
+        <v>524.201416015625</v>
       </c>
       <c r="C315">
-        <v>413.8054809570312</v>
+        <v>521.6325073242188</v>
       </c>
     </row>
     <row r="316" spans="1:3">
@@ -3850,10 +3850,10 @@
         <v>314</v>
       </c>
       <c r="B316">
-        <v>268.9299926757812</v>
+        <v>519.2778930664062</v>
       </c>
       <c r="C316">
-        <v>270.3958435058594</v>
+        <v>507.7131958007812</v>
       </c>
     </row>
     <row r="317" spans="1:3">
@@ -3861,10 +3861,10 @@
         <v>315</v>
       </c>
       <c r="B317">
-        <v>508.331787109375</v>
+        <v>391.4443969726562</v>
       </c>
       <c r="C317">
-        <v>504.0412902832031</v>
+        <v>391.2926635742188</v>
       </c>
     </row>
     <row r="318" spans="1:3">
@@ -3872,10 +3872,10 @@
         <v>316</v>
       </c>
       <c r="B318">
-        <v>484.2152099609375</v>
+        <v>401.9627075195313</v>
       </c>
       <c r="C318">
-        <v>475.7026062011719</v>
+        <v>404.3864440917969</v>
       </c>
     </row>
     <row r="319" spans="1:3">
@@ -3883,10 +3883,10 @@
         <v>317</v>
       </c>
       <c r="B319">
-        <v>416.7562866210937</v>
+        <v>293.0234069824219</v>
       </c>
       <c r="C319">
-        <v>424.9375305175781</v>
+        <v>269.7300109863281</v>
       </c>
     </row>
     <row r="320" spans="1:3">
@@ -3894,10 +3894,10 @@
         <v>318</v>
       </c>
       <c r="B320">
-        <v>293.7619018554688</v>
+        <v>429.3662109375001</v>
       </c>
       <c r="C320">
-        <v>291.5584411621094</v>
+        <v>421.9276123046875</v>
       </c>
     </row>
     <row r="321" spans="1:3">
@@ -3905,10 +3905,10 @@
         <v>319</v>
       </c>
       <c r="B321">
-        <v>574.0115966796875</v>
+        <v>491.2250061035156</v>
       </c>
       <c r="C321">
-        <v>559.2924194335938</v>
+        <v>478.2512512207031</v>
       </c>
     </row>
     <row r="322" spans="1:3">
@@ -3916,10 +3916,10 @@
         <v>320</v>
       </c>
       <c r="B322">
-        <v>371.1893005371094</v>
+        <v>288.747802734375</v>
       </c>
       <c r="C322">
-        <v>374.6272277832031</v>
+        <v>317.0328369140625</v>
       </c>
     </row>
     <row r="323" spans="1:3">
@@ -3927,10 +3927,10 @@
         <v>321</v>
       </c>
       <c r="B323">
-        <v>421.0145874023437</v>
+        <v>520</v>
       </c>
       <c r="C323">
-        <v>406.9107666015625</v>
+        <v>519.7352294921875</v>
       </c>
     </row>
     <row r="324" spans="1:3">
@@ -3938,10 +3938,10 @@
         <v>322</v>
       </c>
       <c r="B324">
-        <v>394.4607849121094</v>
+        <v>285.8371887207031</v>
       </c>
       <c r="C324">
-        <v>403.9319763183594</v>
+        <v>263.0753479003906</v>
       </c>
     </row>
     <row r="325" spans="1:3">
@@ -3949,10 +3949,10 @@
         <v>323</v>
       </c>
       <c r="B325">
-        <v>433.7406921386719</v>
+        <v>303.2987976074219</v>
       </c>
       <c r="C325">
-        <v>433.6092529296875</v>
+        <v>288.8821716308594</v>
       </c>
     </row>
     <row r="326" spans="1:3">
@@ -3960,10 +3960,10 @@
         <v>324</v>
       </c>
       <c r="B326">
-        <v>432.0299987792969</v>
+        <v>386.2344055175781</v>
       </c>
       <c r="C326">
-        <v>428.7540588378906</v>
+        <v>391.3578186035156</v>
       </c>
     </row>
     <row r="327" spans="1:3">
@@ -3971,10 +3971,10 @@
         <v>325</v>
       </c>
       <c r="B327">
-        <v>375.4851989746094</v>
+        <v>392.4024963378906</v>
       </c>
       <c r="C327">
-        <v>407.0546875</v>
+        <v>396.2704162597656</v>
       </c>
     </row>
     <row r="328" spans="1:3">
@@ -3982,10 +3982,10 @@
         <v>326</v>
       </c>
       <c r="B328">
-        <v>403.7326965332032</v>
+        <v>342.2131958007812</v>
       </c>
       <c r="C328">
-        <v>401.8869018554688</v>
+        <v>335.1992797851562</v>
       </c>
     </row>
     <row r="329" spans="1:3">
@@ -3993,10 +3993,10 @@
         <v>327</v>
       </c>
       <c r="B329">
-        <v>574.59619140625</v>
+        <v>427.87451171875</v>
       </c>
       <c r="C329">
-        <v>576.35205078125</v>
+        <v>412.9319458007812</v>
       </c>
     </row>
     <row r="330" spans="1:3">
@@ -4004,10 +4004,10 @@
         <v>328</v>
       </c>
       <c r="B330">
-        <v>396.75</v>
+        <v>253.0278015136719</v>
       </c>
       <c r="C330">
-        <v>398.12841796875</v>
+        <v>249.5642242431641</v>
       </c>
     </row>
     <row r="331" spans="1:3">
@@ -4015,10 +4015,10 @@
         <v>329</v>
       </c>
       <c r="B331">
-        <v>504.4655151367188</v>
+        <v>386.8523864746094</v>
       </c>
       <c r="C331">
-        <v>504.6064758300781</v>
+        <v>377.8785095214844</v>
       </c>
     </row>
     <row r="332" spans="1:3">
@@ -4026,10 +4026,10 @@
         <v>330</v>
       </c>
       <c r="B332">
-        <v>525.80908203125</v>
+        <v>547.0919799804688</v>
       </c>
       <c r="C332">
-        <v>508.1438903808594</v>
+        <v>541.6676635742188</v>
       </c>
     </row>
     <row r="333" spans="1:3">
@@ -4037,10 +4037,10 @@
         <v>331</v>
       </c>
       <c r="B333">
-        <v>271.9433898925781</v>
+        <v>582.230712890625</v>
       </c>
       <c r="C333">
-        <v>267.202392578125</v>
+        <v>582.9131469726562</v>
       </c>
     </row>
     <row r="334" spans="1:3">
@@ -4048,10 +4048,10 @@
         <v>332</v>
       </c>
       <c r="B334">
-        <v>324.5245971679688</v>
+        <v>295.5888977050781</v>
       </c>
       <c r="C334">
-        <v>329.5509948730469</v>
+        <v>271.8855895996094</v>
       </c>
     </row>
     <row r="335" spans="1:3">
@@ -4059,10 +4059,10 @@
         <v>333</v>
       </c>
       <c r="B335">
-        <v>431.1624145507813</v>
+        <v>420.8197021484376</v>
       </c>
       <c r="C335">
-        <v>436.1968078613281</v>
+        <v>411.2798156738281</v>
       </c>
     </row>
     <row r="336" spans="1:3">
@@ -4070,10 +4070,10 @@
         <v>334</v>
       </c>
       <c r="B336">
-        <v>285.8371887207031</v>
+        <v>494.7933044433594</v>
       </c>
       <c r="C336">
-        <v>277.40283203125</v>
+        <v>479.5757751464844</v>
       </c>
     </row>
     <row r="337" spans="1:3">
@@ -4081,10 +4081,10 @@
         <v>335</v>
       </c>
       <c r="B337">
-        <v>398.2799987792969</v>
+        <v>283.4081115722656</v>
       </c>
       <c r="C337">
-        <v>409.7498168945312</v>
+        <v>272.8035888671875</v>
       </c>
     </row>
     <row r="338" spans="1:3">
@@ -4092,10 +4092,10 @@
         <v>336</v>
       </c>
       <c r="B338">
-        <v>358.076904296875</v>
+        <v>274</v>
       </c>
       <c r="C338">
-        <v>375.6535339355469</v>
+        <v>250.9184417724609</v>
       </c>
     </row>
     <row r="339" spans="1:3">
@@ -4103,10 +4103,10 @@
         <v>337</v>
       </c>
       <c r="B339">
-        <v>424.8149108886719</v>
+        <v>392.0159912109376</v>
       </c>
       <c r="C339">
-        <v>435.7645874023438</v>
+        <v>393.21923828125</v>
       </c>
     </row>
     <row r="340" spans="1:3">
@@ -4114,10 +4114,10 @@
         <v>338</v>
       </c>
       <c r="B340">
-        <v>433.8200073242188</v>
+        <v>279.0700073242188</v>
       </c>
       <c r="C340">
-        <v>426.9080810546875</v>
+        <v>270.0424194335938</v>
       </c>
     </row>
     <row r="341" spans="1:3">
@@ -4125,10 +4125,10 @@
         <v>339</v>
       </c>
       <c r="B341">
-        <v>288.747802734375</v>
+        <v>331.0516967773438</v>
       </c>
       <c r="C341">
-        <v>334.8456420898438</v>
+        <v>314.178955078125</v>
       </c>
     </row>
     <row r="342" spans="1:3">
@@ -4136,10 +4136,10 @@
         <v>340</v>
       </c>
       <c r="B342">
-        <v>280.5700073242188</v>
+        <v>492.7901000976562</v>
       </c>
       <c r="C342">
-        <v>284.4444885253906</v>
+        <v>512.1658935546875</v>
       </c>
     </row>
     <row r="343" spans="1:3">
@@ -4147,10 +4147,10 @@
         <v>341</v>
       </c>
       <c r="B343">
-        <v>265.693115234375</v>
+        <v>404.9414978027344</v>
       </c>
       <c r="C343">
-        <v>271.5513610839844</v>
+        <v>397.9496459960938</v>
       </c>
     </row>
     <row r="344" spans="1:3">
@@ -4158,10 +4158,10 @@
         <v>342</v>
       </c>
       <c r="B344">
-        <v>290.7279968261719</v>
+        <v>506.3198852539062</v>
       </c>
       <c r="C344">
-        <v>295.3681945800781</v>
+        <v>509.8775024414062</v>
       </c>
     </row>
     <row r="345" spans="1:3">
@@ -4169,10 +4169,10 @@
         <v>343</v>
       </c>
       <c r="B345">
-        <v>299.4501953125</v>
+        <v>307.4703979492188</v>
       </c>
       <c r="C345">
-        <v>297.1859436035156</v>
+        <v>291.9646606445312</v>
       </c>
     </row>
     <row r="346" spans="1:3">
@@ -4180,10 +4180,10 @@
         <v>344</v>
       </c>
       <c r="B346">
-        <v>404.9414978027344</v>
+        <v>339.4797058105469</v>
       </c>
       <c r="C346">
-        <v>408.1109313964844</v>
+        <v>335.4169006347656</v>
       </c>
     </row>
     <row r="347" spans="1:3">
@@ -4191,10 +4191,10 @@
         <v>345</v>
       </c>
       <c r="B347">
-        <v>395.1661071777344</v>
+        <v>406.2496948242187</v>
       </c>
       <c r="C347">
-        <v>397.7311706542969</v>
+        <v>410.4089965820312</v>
       </c>
     </row>
     <row r="348" spans="1:3">
@@ -4202,10 +4202,10 @@
         <v>346</v>
       </c>
       <c r="B348">
-        <v>522.7183227539062</v>
+        <v>326.4010009765625</v>
       </c>
       <c r="C348">
-        <v>506.7522583007812</v>
+        <v>311.1178894042969</v>
       </c>
     </row>
     <row r="349" spans="1:3">
@@ -4213,10 +4213,10 @@
         <v>347</v>
       </c>
       <c r="B349">
-        <v>371.7095031738281</v>
+        <v>426.8922119140624</v>
       </c>
       <c r="C349">
-        <v>376.8969116210938</v>
+        <v>414.0775756835938</v>
       </c>
     </row>
     <row r="350" spans="1:3">
@@ -4224,10 +4224,10 @@
         <v>348</v>
       </c>
       <c r="B350">
-        <v>246.5</v>
+        <v>432.9602050781251</v>
       </c>
       <c r="C350">
-        <v>264.1055908203125</v>
+        <v>418.2557373046875</v>
       </c>
     </row>
     <row r="351" spans="1:3">
@@ -4235,10 +4235,10 @@
         <v>349</v>
       </c>
       <c r="B351">
-        <v>398.5882873535156</v>
+        <v>288.618408203125</v>
       </c>
       <c r="C351">
-        <v>407.5635375976562</v>
+        <v>267.4600219726562</v>
       </c>
     </row>
     <row r="352" spans="1:3">
@@ -4246,10 +4246,153 @@
         <v>350</v>
       </c>
       <c r="B352">
-        <v>422.3388977050781</v>
+        <v>494.9695129394531</v>
       </c>
       <c r="C352">
-        <v>405.7422485351562</v>
+        <v>489.3559265136719</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3">
+      <c r="A353" s="1">
+        <v>351</v>
+      </c>
+      <c r="B353">
+        <v>398.1430969238281</v>
+      </c>
+      <c r="C353">
+        <v>395.9058532714844</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3">
+      <c r="A354" s="1">
+        <v>352</v>
+      </c>
+      <c r="B354">
+        <v>266.2799072265625</v>
+      </c>
+      <c r="C354">
+        <v>253.3387756347656</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3">
+      <c r="A355" s="1">
+        <v>353</v>
+      </c>
+      <c r="B355">
+        <v>312.4585876464844</v>
+      </c>
+      <c r="C355">
+        <v>318.9342651367188</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3">
+      <c r="A356" s="1">
+        <v>354</v>
+      </c>
+      <c r="B356">
+        <v>429.4544067382812</v>
+      </c>
+      <c r="C356">
+        <v>411.9880065917969</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3">
+      <c r="A357" s="1">
+        <v>355</v>
+      </c>
+      <c r="B357">
+        <v>569.57177734375</v>
+      </c>
+      <c r="C357">
+        <v>578.4328002929688</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3">
+      <c r="A358" s="1">
+        <v>356</v>
+      </c>
+      <c r="B358">
+        <v>396.2379150390625</v>
+      </c>
+      <c r="C358">
+        <v>392.9199523925781</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3">
+      <c r="A359" s="1">
+        <v>357</v>
+      </c>
+      <c r="B359">
+        <v>419.1980895996094</v>
+      </c>
+      <c r="C359">
+        <v>416.9684143066406</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3">
+      <c r="A360" s="1">
+        <v>358</v>
+      </c>
+      <c r="B360">
+        <v>305.5209045410156</v>
+      </c>
+      <c r="C360">
+        <v>299.460205078125</v>
+      </c>
+    </row>
+    <row r="361" spans="1:3">
+      <c r="A361" s="1">
+        <v>359</v>
+      </c>
+      <c r="B361">
+        <v>303.418701171875</v>
+      </c>
+      <c r="C361">
+        <v>276.8084106445312</v>
+      </c>
+    </row>
+    <row r="362" spans="1:3">
+      <c r="A362" s="1">
+        <v>360</v>
+      </c>
+      <c r="B362">
+        <v>369.7710876464844</v>
+      </c>
+      <c r="C362">
+        <v>366.77685546875</v>
+      </c>
+    </row>
+    <row r="363" spans="1:3">
+      <c r="A363" s="1">
+        <v>361</v>
+      </c>
+      <c r="B363">
+        <v>229.1065063476562</v>
+      </c>
+      <c r="C363">
+        <v>254.5089111328125</v>
+      </c>
+    </row>
+    <row r="364" spans="1:3">
+      <c r="A364" s="1">
+        <v>362</v>
+      </c>
+      <c r="B364">
+        <v>586.73828125</v>
+      </c>
+      <c r="C364">
+        <v>579.6929321289062</v>
+      </c>
+    </row>
+    <row r="365" spans="1:3">
+      <c r="A365" s="1">
+        <v>363</v>
+      </c>
+      <c r="B365">
+        <v>268.9299926757812</v>
+      </c>
+      <c r="C365">
+        <v>252.9957580566406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>